<commit_message>
Update progparser.py and tabconv.py
</commit_message>
<xml_diff>
--- a/usr/share/python/prog_parser_sample/reg_table.xlsx
+++ b/usr/share/python/prog_parser_sample/reg_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -321,12 +321,9 @@
   <si>
     <t xml:space="preserve">SRC1_A4X4_UPSAMPLE_MODE
 0: A8
-1: {A4
-4'h0}
-2: {A4
-4'h4}
-3: {A4
-4bit A4[0]}</t>
+1: {A4, 4'h0}
+2: {A4, 4'h4}
+3: {A4, 4bit A4[0]}</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
@@ -368,18 +365,12 @@
     <t xml:space="preserve">0x24</t>
   </si>
   <si>
-    <t xml:space="preserve">0x10</t>
-  </si>
-  <si>
     <t xml:space="preserve">3_0</t>
   </si>
   <si>
     <t xml:space="preserve">REG_SET1_VAR1</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
     <t xml:space="preserve">7_4</t>
   </si>
   <si>
@@ -447,6 +438,15 @@
   </si>
   <si>
     <t xml:space="preserve">REG_SET3_VAR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5a5aa5a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REG_ADDR2</t>
   </si>
   <si>
     <t xml:space="preserve">0x40</t>
@@ -474,6 +474,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -495,6 +496,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -515,6 +517,7 @@
       <color rgb="FF808080"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -526,6 +529,7 @@
       <sz val="12"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -607,7 +611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -653,6 +657,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,6 +677,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,6 +702,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -821,17 +837,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F49" activeCellId="0" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="37.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="6.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="7.91"/>
@@ -840,7 +857,7 @@
     <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="3"/>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -854,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
         <v>2</v>
@@ -868,6 +885,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
@@ -878,6 +896,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
@@ -885,6 +904,7 @@
     </row>
     <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
@@ -900,875 +920,894 @@
       <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" s="18" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" s="20" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="C7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="21" t="s">
+      <c r="F7" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="F8" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="F9" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="F10" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="F11" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="F12" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" s="30" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+    <row r="14" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="F14" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="25" t="s">
+      <c r="C15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="F15" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="F16" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" s="30" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="F17" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" s="33" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" s="30" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="F18" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" s="33" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="F19" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="F20" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="F21" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="21" t="s">
+      <c r="F22" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" s="30" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="F23" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" s="33" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" s="30" customFormat="true" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="21" t="s">
+      <c r="F24" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" s="33" customFormat="true" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" s="27" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
+      <c r="F25" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" s="30" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="21" t="s">
+      <c r="F26" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" s="30" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="F27" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" s="33" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" s="30" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="F28" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" s="33" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="21" t="s">
+      <c r="F29" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="21" t="s">
+      <c r="F30" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="21" t="s">
+      <c r="F31" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="21" t="s">
+      <c r="F32" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="21" t="s">
+      <c r="F33" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="21" t="s">
+      <c r="F34" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
+      <c r="F35" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" s="30" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="15" t="s">
+      <c r="C36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="21" t="s">
+      <c r="F36" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F37" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="21" t="s">
+      <c r="F37" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="21" t="s">
+      <c r="F38" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" s="30" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="21" t="s">
+      <c r="F39" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" s="33" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="F40" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" s="30" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="21" t="s">
+      <c r="F40" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" s="33" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="21"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="21" t="s">
+      <c r="F41" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="21" t="s">
+      <c r="F42" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="21" t="s">
+      <c r="F43" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="19"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="21" t="s">
+      <c r="F44" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="21"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="21" t="s">
+      <c r="F45" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="21" t="s">
+      <c r="F46" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="13" t="s">
+      <c r="F47" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" s="30" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="15" t="s">
+      <c r="B48" s="15"/>
+      <c r="C48" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="E48" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="F48" s="29" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F48" s="26" t="s">
+      <c r="E49" s="31" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="49" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" s="21" t="s">
+      <c r="F49" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E49" s="28" t="s">
+    </row>
+    <row r="50" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="21"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="D50" s="24" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="50" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="19"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="21" t="s">
+      <c r="E50" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="F50" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="E50" s="28" t="s">
+    </row>
+    <row r="51" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="D51" s="24" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="51" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="19"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="21" t="s">
+      <c r="E51" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="F51" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" s="30" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="B52" s="15"/>
+      <c r="C52" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="s">
+      <c r="D52" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="15" t="s">
+      <c r="E52" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="F52" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="D53" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E53" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="F52" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="19"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="21" t="s">
+      <c r="F53" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" s="33" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="21"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E53" s="28" t="s">
+      <c r="D54" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" s="30" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="19"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="21" t="s">
+      <c r="F54" s="32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" s="27" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="21"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="E54" s="28" t="s">
+      <c r="D55" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="19"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="21" t="s">
+      <c r="F55" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="D55" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E55" s="22" t="s">
+    </row>
+    <row r="56" s="30" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="F55" s="23" t="s">
+      <c r="B56" s="15"/>
+      <c r="C56" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="28" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="56" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="13" t="s">
+      <c r="F56" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" s="30" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="15" t="s">
+      <c r="B57" s="15"/>
+      <c r="C57" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D57" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="s">
+      <c r="E57" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="F57" s="29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" s="20" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C57" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="15" t="s">
+      <c r="B58" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E57" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" s="32" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="32" t="s">
+      <c r="E58" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
+      <c r="F58" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" s="35" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>